<commit_message>
tambahan spec baru konfirmasi pembayaran
tambahan spec baru konfirmasi pembayaran
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Transaksi" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>MST005</t>
+  </si>
+  <si>
+    <t>TRX001</t>
+  </si>
+  <si>
+    <t>Konfirmasi Pembayaran</t>
   </si>
 </sst>
 </file>
@@ -392,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,12 +463,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
tambah table master agent
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Konfirmasi Pembayaran</t>
+  </si>
+  <si>
+    <t>master agent</t>
+  </si>
+  <si>
+    <t>MST010</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +462,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -466,13 +480,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,10 +498,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penambahan order boking spec
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>MST010</t>
+  </si>
+  <si>
+    <t>Header Booking Order</t>
+  </si>
+  <si>
+    <t>TRX010</t>
+  </si>
+  <si>
+    <t>Detail Booking Order</t>
+  </si>
+  <si>
+    <t>TRX011</t>
+  </si>
+  <si>
+    <t>Detail Pembayaran -  Booking Order</t>
+  </si>
+  <si>
+    <t>TRX012</t>
   </si>
 </sst>
 </file>
@@ -477,15 +495,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,6 +521,30 @@
       </c>
       <c r="B2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penambahan table log dan spec
ada perubahan di table trx010, trx011 dan ada penambahan table log001.
di spec juga ada penambahan
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="Transaksi" sheetId="2" r:id="rId2"/>
     <sheet name="saldo" sheetId="3" r:id="rId3"/>
+    <sheet name="Log" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>BLNC001</t>
+  </si>
+  <si>
+    <t>LOG001</t>
+  </si>
+  <si>
+    <t>Log Deposit</t>
   </si>
 </sst>
 </file>
@@ -562,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,4 +598,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
penambahan temp table untuk api hotel
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="Transaksi" sheetId="2" r:id="rId2"/>
     <sheet name="saldo" sheetId="3" r:id="rId3"/>
     <sheet name="Log" sheetId="4" r:id="rId4"/>
+    <sheet name="Temp" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -95,6 +96,18 @@
   </si>
   <si>
     <t>Log Deposit</t>
+  </si>
+  <si>
+    <t>temp001</t>
+  </si>
+  <si>
+    <t>Kode table</t>
+  </si>
+  <si>
+    <t>nama Table</t>
+  </si>
+  <si>
+    <t>Temp Header Hotel API</t>
   </si>
 </sst>
 </file>
@@ -604,18 +617,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -624,6 +637,41 @@
       </c>
       <c r="B2" t="s">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tambahan temp table api hotel
tambahan temp table api hotel
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Temp Header Hotel API</t>
+  </si>
+  <si>
+    <t>tem002</t>
+  </si>
+  <si>
+    <t>temp detail rate hotel API</t>
   </si>
 </sst>
 </file>
@@ -646,10 +652,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +680,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
temp table berubah bknya
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>temp detail rate hotel API</t>
+  </si>
+  <si>
+    <t>master Hotel</t>
+  </si>
+  <si>
+    <t>MST020</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +524,14 @@
       </c>
       <c r="B7" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
perubahan spec room type dan detail room serta table
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>MST021</t>
+  </si>
+  <si>
+    <t>master  room rate</t>
+  </si>
+  <si>
+    <t>MST023</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,10 +562,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penambahan field di mst022
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>master fasilitas kamar</t>
+  </si>
+  <si>
+    <t>BLNC010</t>
+  </si>
+  <si>
+    <t>Saldo Hutang Cancel Booking</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -682,10 +688,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,6 +730,14 @@
       </c>
       <c r="B4" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penambahan query di list hotel
lihat yg kuning2 di list hotel
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>Saldo Hutang Cancel Booking</t>
+  </si>
+  <si>
+    <t>Detail summary order</t>
+  </si>
+  <si>
+    <t>TRX013</t>
+  </si>
+  <si>
+    <t>Saldo Booking Order Detail - summary</t>
+  </si>
+  <si>
+    <t>BLNC004</t>
   </si>
 </sst>
 </file>
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +679,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -679,6 +691,14 @@
       </c>
       <c r="B5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -688,10 +708,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +738,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -726,17 +746,25 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update query search detail room
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>BLNC004</t>
+  </si>
+  <si>
+    <t>temp003</t>
+  </si>
+  <si>
+    <t>temp table search detail room rate</t>
+  </si>
+  <si>
+    <t>tem004</t>
   </si>
 </sst>
 </file>
@@ -710,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -806,10 +815,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,6 +851,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
spec baru untuk agent
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>tem004</t>
+  </si>
+  <si>
+    <t>BLNC020</t>
+  </si>
+  <si>
+    <t>Saldo Deposit Agent</t>
   </si>
 </sst>
 </file>
@@ -717,10 +723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +781,14 @@
       </c>
       <c r="B6" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tambah spec n log
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Master" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Transaksi" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="saldo" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Log" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Temp" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Transaksi" sheetId="2" r:id="rId2"/>
+    <sheet name="saldo" sheetId="3" r:id="rId3"/>
+    <sheet name="Log" sheetId="4" r:id="rId4"/>
+    <sheet name="Temp" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -243,9 +242,6 @@
     <t>nama Table</t>
   </si>
   <si>
-    <t>LOG001</t>
-  </si>
-  <si>
     <t>Log Deposit</t>
   </si>
   <si>
@@ -271,37 +267,22 @@
   </si>
   <si>
     <t>tem004</t>
+  </si>
+  <si>
+    <t>LOG010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -313,7 +294,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -321,535 +302,757 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col min="1" max="1" width="19"/>
+    <col min="2" max="2" width="10.5703125"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col min="1" max="1" width="32.28515625"/>
+    <col min="2" max="2" width="21.85546875"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col min="1" max="1" width="28.140625"/>
+    <col min="2" max="2" width="10.5703125"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col min="1" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>76</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col min="1" max="1" width="10.28515625"/>
+    <col min="2" max="2" width="10.85546875"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="0" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="0" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>82</v>
+      <c r="B5" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
penambahan spec log dan query allotment
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t>LOG010</t>
+  </si>
+  <si>
+    <t>LOG020</t>
+  </si>
+  <si>
+    <t>log allotment</t>
   </si>
 </sst>
 </file>
@@ -957,10 +963,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,6 +994,14 @@
       </c>
       <c r="C2" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spec cancel sama agent menu
</commit_message>
<xml_diff>
--- a/document/file ormat.xlsx
+++ b/document/file ormat.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Nama Tabel</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>log allotment</t>
+  </si>
+  <si>
+    <t>LOG030</t>
+  </si>
+  <si>
+    <t>log cancel</t>
   </si>
 </sst>
 </file>
@@ -963,10 +969,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,6 +1008,14 @@
       </c>
       <c r="B3" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>